<commit_message>
V 0.1.7/h2 Auto Login bug: fixed
</commit_message>
<xml_diff>
--- a/Assets/Resources/Items/AdvancedItemData.xlsx
+++ b/Assets/Resources/Items/AdvancedItemData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="70">
   <si>
     <t>PartName</t>
   </si>
@@ -130,12 +130,6 @@
     <t>Walther_MRS_reflex_sight</t>
   </si>
   <si>
-    <t>MainItemName</t>
-  </si>
-  <si>
-    <t>NecessaryItemNames</t>
-  </si>
-  <si>
     <t>Textures/ItemTextures/TEST/TestBack</t>
   </si>
   <si>
@@ -212,6 +206,30 @@
   </si>
   <si>
     <t>AKS-74U_Zenit_B-11_handguard;AKS-74U_Wooden_handguard</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>SystemName</t>
+  </si>
+  <si>
+    <t>ItemName</t>
+  </si>
+  <si>
+    <t>WeaponMain</t>
+  </si>
+  <si>
+    <t>NecessaryTypes</t>
+  </si>
+  <si>
+    <t>Grip;Handguard;WeaponBody</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>This is a sovjet AKS-74U carabine</t>
   </si>
 </sst>
 </file>
@@ -475,7 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -523,7 +541,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -552,7 +570,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -677,7 +695,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
@@ -730,7 +748,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
@@ -759,7 +777,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>10</v>
@@ -788,7 +806,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
@@ -817,7 +835,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>10</v>
@@ -846,7 +864,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>10</v>
@@ -898,7 +916,7 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>10</v>
@@ -907,7 +925,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F16" s="1">
         <v>205</v>
@@ -930,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F17" s="1">
         <v>535</v>
@@ -1042,7 +1060,7 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>10</v>
@@ -1074,7 +1092,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F23" s="1">
         <v>62</v>
@@ -1091,10 +1109,10 @@
     </row>
     <row r="24" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>10</v>
@@ -1120,10 +1138,10 @@
     </row>
     <row r="25" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>10</v>
@@ -1152,7 +1170,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>10</v>
@@ -1181,7 +1199,7 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>10</v>
@@ -1210,7 +1228,7 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>10</v>
@@ -1239,7 +1257,7 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>10</v>
@@ -1265,10 +1283,10 @@
     </row>
     <row r="30" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>10</v>
@@ -1297,7 +1315,7 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>10</v>
@@ -1326,7 +1344,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>10</v>
@@ -1355,7 +1373,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>10</v>
@@ -1407,7 +1425,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>10</v>
@@ -2403,49 +2421,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="29" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
V 0.1.7/i2 Dev Consol Admin and Consold True Dependency
</commit_message>
<xml_diff>
--- a/Assets/Resources/Items/AdvancedItemData.xlsx
+++ b/Assets/Resources/Items/AdvancedItemData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="71">
   <si>
     <t>PartName</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>This is a sovjet AKS-74U carabine</t>
+  </si>
+  <si>
+    <t>ConnectedItem</t>
   </si>
 </sst>
 </file>
@@ -493,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I999"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -2421,10 +2424,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2434,7 +2437,7 @@
     <col min="6" max="29" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>64</v>
       </c>
@@ -2450,8 +2453,11 @@
       <c r="E1" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>60</v>
       </c>
@@ -2467,21 +2473,24 @@
       <c r="E2" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
V 0.1.7/k2 SP points: added , MainItem Handling: updated , TestPlayer rePlaced by Admin , SectorScale increased to 1.3f , AdvancedItem fitter bug: fixed
</commit_message>
<xml_diff>
--- a/Assets/Resources/Items/AdvancedItemData.xlsx
+++ b/Assets/Resources/Items/AdvancedItemData.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
-    <sheet name="Munka2" sheetId="2" r:id="rId2"/>
+    <sheet name="AdvancedItems" sheetId="1" r:id="rId1"/>
+    <sheet name="MainItems" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
   <si>
     <t>PartName</t>
   </si>
@@ -49,45 +49,21 @@
     <t>Y2</t>
   </si>
   <si>
-    <t>TestBack</t>
-  </si>
-  <si>
     <t>CP0</t>
   </si>
   <si>
-    <t>TestBox</t>
-  </si>
-  <si>
-    <t>TestCenter</t>
-  </si>
-  <si>
     <t>CP1</t>
   </si>
   <si>
-    <t>TestUpper</t>
-  </si>
-  <si>
     <t>CP2</t>
   </si>
   <si>
-    <t>TestButtom</t>
-  </si>
-  <si>
     <t>CP3</t>
   </si>
   <si>
-    <t>TestFront</t>
-  </si>
-  <si>
     <t>CP4</t>
   </si>
   <si>
-    <t>TestFoot</t>
-  </si>
-  <si>
-    <t>TestHead</t>
-  </si>
-  <si>
     <t>AK-74_5.45x39_6L20_30-round_magasine</t>
   </si>
   <si>
@@ -130,30 +106,6 @@
     <t>Walther_MRS_reflex_sight</t>
   </si>
   <si>
-    <t>Textures/ItemTextures/TEST/TestBack</t>
-  </si>
-  <si>
-    <t>Textures/ItemTextures/TEST/TestBox</t>
-  </si>
-  <si>
-    <t>Textures/ItemTextures/TEST/TestButtom</t>
-  </si>
-  <si>
-    <t>Textures/ItemTextures/TEST/TestCenter</t>
-  </si>
-  <si>
-    <t>Textures/ItemTextures/TEST/TestFoot</t>
-  </si>
-  <si>
-    <t>Textures/ItemTextures/TEST/TestFront</t>
-  </si>
-  <si>
-    <t>Textures/ItemTextures/TEST/TestHead</t>
-  </si>
-  <si>
-    <t>Textures/ItemTextures/TEST/TestUpper</t>
-  </si>
-  <si>
     <t>Textures/ItemTextures/Weapons/Bodys/AKS-74U_Body</t>
   </si>
   <si>
@@ -233,6 +185,21 @@
   </si>
   <si>
     <t>ConnectedItem</t>
+  </si>
+  <si>
+    <t>PointType</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -273,12 +240,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -494,977 +460,704 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I999"/>
+  <dimension ref="A1:J985"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" customWidth="1"/>
-    <col min="6" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="27" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1">
+        <v>205</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45</v>
+      </c>
+      <c r="I2" s="1">
+        <v>205</v>
+      </c>
+      <c r="J2" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1">
+        <v>535</v>
+      </c>
+      <c r="H3" s="1">
+        <v>99</v>
+      </c>
+      <c r="I3" s="1">
+        <v>533</v>
+      </c>
+      <c r="J3" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1">
+        <v>285</v>
+      </c>
+      <c r="H4" s="1">
+        <v>128</v>
+      </c>
+      <c r="I4" s="1">
+        <v>371</v>
+      </c>
+      <c r="J4" s="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1">
+        <v>453</v>
+      </c>
+      <c r="H5" s="1">
+        <v>137</v>
+      </c>
+      <c r="I5" s="1">
+        <v>516</v>
+      </c>
+      <c r="J5" s="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="1">
+        <v>56</v>
+      </c>
+      <c r="H6" s="1">
+        <v>81</v>
+      </c>
+      <c r="I6" s="1">
+        <v>56</v>
+      </c>
+      <c r="J6" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2">
+        <v>312</v>
+      </c>
+      <c r="H7" s="2">
+        <v>87</v>
+      </c>
+      <c r="I7" s="2">
+        <v>535</v>
+      </c>
+      <c r="J7" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="1">
+        <v>196</v>
+      </c>
+      <c r="H9" s="1">
+        <v>30</v>
+      </c>
+      <c r="I9" s="1">
+        <v>196</v>
+      </c>
+      <c r="J9" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="1">
+        <v>62</v>
+      </c>
+      <c r="H10" s="1">
+        <v>161</v>
+      </c>
+      <c r="I10" s="1">
+        <v>132</v>
+      </c>
+      <c r="J10" s="1">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="1">
+        <v>215</v>
+      </c>
+      <c r="H11" s="1">
+        <v>54</v>
+      </c>
+      <c r="I11" s="1">
+        <v>215</v>
+      </c>
+      <c r="J11" s="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="1">
+        <v>62</v>
+      </c>
+      <c r="H12" s="1">
+        <v>87</v>
+      </c>
+      <c r="I12" s="1">
+        <v>60</v>
+      </c>
+      <c r="J12" s="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1">
+        <v>112</v>
+      </c>
+      <c r="H13" s="1">
+        <v>12</v>
+      </c>
+      <c r="I13" s="1">
+        <v>246</v>
+      </c>
+      <c r="J13" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="1">
+        <v>103</v>
+      </c>
+      <c r="H14" s="1">
+        <v>9</v>
+      </c>
+      <c r="I14" s="1">
+        <v>225</v>
+      </c>
+      <c r="J14" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="1">
+        <v>21</v>
+      </c>
+      <c r="H15" s="1">
+        <v>19</v>
+      </c>
+      <c r="I15" s="1">
+        <v>112</v>
+      </c>
+      <c r="J15" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="1">
+        <v>14</v>
+      </c>
+      <c r="H16" s="1">
+        <v>9</v>
+      </c>
+      <c r="I16" s="1">
+        <v>116</v>
+      </c>
+      <c r="J16" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1">
+        <v>18</v>
+      </c>
+      <c r="H17" s="1">
+        <v>26</v>
+      </c>
+      <c r="I17" s="1">
+        <v>89</v>
+      </c>
+      <c r="J17" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="1">
+        <v>138</v>
+      </c>
+      <c r="H18" s="1">
+        <v>12</v>
+      </c>
+      <c r="I18" s="1">
+        <v>138</v>
+      </c>
+      <c r="J18" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="2">
+        <v>102</v>
+      </c>
+      <c r="H19" s="2">
+        <v>97</v>
+      </c>
+      <c r="I19" s="2">
+        <v>436</v>
+      </c>
+      <c r="J19" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="2">
+        <v>105</v>
+      </c>
+      <c r="H20" s="2">
+        <v>97</v>
+      </c>
+      <c r="I20" s="2">
+        <v>443</v>
+      </c>
+      <c r="J20" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E21" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="F21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="2">
+        <v>180</v>
+      </c>
+      <c r="H21" s="2">
+        <v>32</v>
+      </c>
+      <c r="I21" s="2">
+        <v>288</v>
+      </c>
+      <c r="J21" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0</v>
-      </c>
-      <c r="I2" s="4">
-        <v>0</v>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="2">
+        <v>6</v>
+      </c>
+      <c r="H22" s="2">
+        <v>95</v>
+      </c>
+      <c r="I22" s="2">
+        <v>115</v>
+      </c>
+      <c r="J22" s="2">
+        <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1552</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1090</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1956</v>
-      </c>
-      <c r="I3" s="4">
-        <v>1495</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1524</v>
-      </c>
-      <c r="G10" s="4">
-        <v>424</v>
-      </c>
-      <c r="H10" s="4">
-        <v>2618</v>
-      </c>
-      <c r="I10" s="4">
-        <v>1515</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="1">
-        <v>205</v>
-      </c>
-      <c r="G16" s="1">
-        <v>45</v>
-      </c>
-      <c r="H16" s="1">
-        <v>205</v>
-      </c>
-      <c r="I16" s="1">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="1">
-        <v>535</v>
-      </c>
-      <c r="G17" s="1">
-        <v>99</v>
-      </c>
-      <c r="H17" s="1">
-        <v>533</v>
-      </c>
-      <c r="I17" s="1">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="1">
-        <v>285</v>
-      </c>
-      <c r="G18" s="1">
-        <v>128</v>
-      </c>
-      <c r="H18" s="1">
-        <v>371</v>
-      </c>
-      <c r="I18" s="1">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="1">
-        <v>453</v>
-      </c>
-      <c r="G19" s="1">
-        <v>137</v>
-      </c>
-      <c r="H19" s="1">
-        <v>516</v>
-      </c>
-      <c r="I19" s="1">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="1">
-        <v>56</v>
-      </c>
-      <c r="G20" s="1">
-        <v>81</v>
-      </c>
-      <c r="H20" s="1">
-        <v>56</v>
-      </c>
-      <c r="I20" s="1">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="2">
-        <v>312</v>
-      </c>
-      <c r="G21" s="2">
-        <v>87</v>
-      </c>
-      <c r="H21" s="2">
-        <v>535</v>
-      </c>
-      <c r="I21" s="2">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="1">
-        <v>196</v>
-      </c>
-      <c r="G22" s="1">
-        <v>30</v>
-      </c>
-      <c r="H22" s="1">
-        <v>196</v>
-      </c>
-      <c r="I22" s="1">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" s="1">
-        <v>62</v>
-      </c>
-      <c r="G23" s="1">
-        <v>161</v>
-      </c>
-      <c r="H23" s="1">
-        <v>132</v>
-      </c>
-      <c r="I23" s="1">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="1">
-        <v>215</v>
-      </c>
-      <c r="G24" s="1">
-        <v>54</v>
-      </c>
-      <c r="H24" s="1">
-        <v>215</v>
-      </c>
-      <c r="I24" s="1">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" s="1">
-        <v>62</v>
-      </c>
-      <c r="G25" s="1">
-        <v>87</v>
-      </c>
-      <c r="H25" s="1">
-        <v>60</v>
-      </c>
-      <c r="I25" s="1">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="1">
-        <v>112</v>
-      </c>
-      <c r="G26" s="1">
-        <v>12</v>
-      </c>
-      <c r="H26" s="1">
-        <v>246</v>
-      </c>
-      <c r="I26" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="1">
-        <v>103</v>
-      </c>
-      <c r="G27" s="1">
-        <v>9</v>
-      </c>
-      <c r="H27" s="1">
-        <v>225</v>
-      </c>
-      <c r="I27" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="1">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="1">
-        <v>21</v>
-      </c>
-      <c r="G28" s="1">
-        <v>19</v>
-      </c>
-      <c r="H28" s="1">
-        <v>112</v>
-      </c>
-      <c r="I28" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F29" s="1">
-        <v>14</v>
-      </c>
-      <c r="G29" s="1">
-        <v>9</v>
-      </c>
-      <c r="H29" s="1">
-        <v>116</v>
-      </c>
-      <c r="I29" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30" s="1">
-        <v>18</v>
-      </c>
-      <c r="G30" s="1">
-        <v>26</v>
-      </c>
-      <c r="H30" s="1">
-        <v>89</v>
-      </c>
-      <c r="I30" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" s="1">
-        <v>138</v>
-      </c>
-      <c r="G31" s="1">
-        <v>12</v>
-      </c>
-      <c r="H31" s="1">
-        <v>138</v>
-      </c>
-      <c r="I31" s="1">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F32" s="2">
-        <v>102</v>
-      </c>
-      <c r="G32" s="2">
-        <v>97</v>
-      </c>
-      <c r="H32" s="2">
-        <v>436</v>
-      </c>
-      <c r="I32" s="2">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="2">
-        <v>105</v>
-      </c>
-      <c r="G33" s="2">
-        <v>97</v>
-      </c>
-      <c r="H33" s="2">
-        <v>443</v>
-      </c>
-      <c r="I33" s="2">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0</v>
-      </c>
-      <c r="E34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" s="2">
-        <v>180</v>
-      </c>
-      <c r="G34" s="2">
-        <v>32</v>
-      </c>
-      <c r="H34" s="2">
-        <v>288</v>
-      </c>
-      <c r="I34" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0</v>
-      </c>
-      <c r="E35" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="2">
-        <v>6</v>
-      </c>
-      <c r="G35" s="2">
-        <v>95</v>
-      </c>
-      <c r="H35" s="2">
-        <v>115</v>
-      </c>
-      <c r="I35" s="2">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2402,20 +2095,6 @@
     <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2426,7 +2105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -2439,42 +2118,42 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
V 0.1.7/o2 Player Character flip: fixed
</commit_message>
<xml_diff>
--- a/Assets/Resources/Items/AdvancedItemData.xlsx
+++ b/Assets/Resources/Items/AdvancedItemData.xlsx
@@ -9,18 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="AdvancedItems" sheetId="1" r:id="rId1"/>
+    <sheet name="PartDatas" sheetId="1" r:id="rId1"/>
     <sheet name="MainItems" sheetId="2" r:id="rId2"/>
+    <sheet name="AdvancedItems" sheetId="3" r:id="rId3"/>
+    <sheet name="System" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="133">
   <si>
     <t>PartName</t>
   </si>
@@ -67,21 +69,12 @@
     <t>AK-74_5.45x39_6L20_30-round_magasine</t>
   </si>
   <si>
-    <t>AK-74_5.45x39_6L20_30-round_magasine;AK-74_5.45x39_6L31_60-round_magasine</t>
-  </si>
-  <si>
-    <t>AK_Zenit_RK-3_pistol_grip;AKS-74U_bakelite_pistol_grip</t>
-  </si>
-  <si>
     <t>CP5</t>
   </si>
   <si>
     <t>AK-105_5.45x39_muzzle_brake-compensator</t>
   </si>
   <si>
-    <t>AKS-74U_dust_cover;AKS-74U_Legal_Arsenal_Pilgrim_railed_dust_cover</t>
-  </si>
-  <si>
     <t>AKS-74U_Zenit_B-11_handguard</t>
   </si>
   <si>
@@ -157,9 +150,6 @@
     <t>AKS-74U</t>
   </si>
   <si>
-    <t>AKS-74U_Zenit_B-11_handguard;AKS-74U_Wooden_handguard</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -175,9 +165,6 @@
     <t>NecessaryTypes</t>
   </si>
   <si>
-    <t>Grip;Handguard;WeaponBody</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -200,13 +187,247 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Glock_19X_9x19_pistol_body</t>
+  </si>
+  <si>
+    <t>Glock_9x19_19-round_magasine_(Coyote)</t>
+  </si>
+  <si>
+    <t>Glock_19X_9x19_barrel</t>
+  </si>
+  <si>
+    <t>Glock_19X_pistol_slide</t>
+  </si>
+  <si>
+    <t>Olight_Baldr_Pro_tactical_flashlight_with_laser_(tan)</t>
+  </si>
+  <si>
+    <t>Glock_19X_front_sight</t>
+  </si>
+  <si>
+    <t>Glock_19X_rear_sight</t>
+  </si>
+  <si>
+    <t>Textures/ItemTextures/Weapons/Sights/Glock_19X_front_sight</t>
+  </si>
+  <si>
+    <t>Textures/ItemTextures/Weapons/Sights/Glock_19X_rear_sight</t>
+  </si>
+  <si>
+    <t>Textures/ItemTextures/Weapons/Bodys/Glock_19X_9x19_pistol_body</t>
+  </si>
+  <si>
+    <t>Textures/ItemTextures/Weapons/Magasines/Glock_9x19_19-round_magasine_(Coyote)</t>
+  </si>
+  <si>
+    <t>Textures/ItemTextures/Weapons/Lasers/Olight_Baldr_Pro_tactical_flashlight_with_laser_(tan)</t>
+  </si>
+  <si>
+    <t>Textures/ItemTextures/Weapons/Barrels/Glock_19X_9x19_barrel</t>
+  </si>
+  <si>
+    <t>Textures/ItemTextures/Weapons/Slides/Glock_19X_pistol_slide</t>
+  </si>
+  <si>
+    <t>SystemNames</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>SizeX</t>
+  </si>
+  <si>
+    <t>SizeY</t>
+  </si>
+  <si>
+    <t>IsDropAble</t>
+  </si>
+  <si>
+    <t>IsRemoveAble</t>
+  </si>
+  <si>
+    <t>IsUnloadAble</t>
+  </si>
+  <si>
+    <t>IsModificationAble</t>
+  </si>
+  <si>
+    <t>SizeChanger</t>
+  </si>
+  <si>
+    <t>IsOpenAble</t>
+  </si>
+  <si>
+    <t>ContainerPath</t>
+  </si>
+  <si>
+    <t>MaxStackSize</t>
+  </si>
+  <si>
+    <t>MagasineSize</t>
+  </si>
+  <si>
+    <t>Spread</t>
+  </si>
+  <si>
+    <t>Fpm</t>
+  </si>
+  <si>
+    <t>Recoil</t>
+  </si>
+  <si>
+    <t>Accturacy</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Ergonomy</t>
+  </si>
+  <si>
+    <t>Caliber</t>
+  </si>
+  <si>
+    <t>UseLeft</t>
+  </si>
+  <si>
+    <t>AKS-74U DC</t>
+  </si>
+  <si>
+    <t>Types</t>
+  </si>
+  <si>
+    <t>Dustcover</t>
+  </si>
+  <si>
+    <t>Grip</t>
+  </si>
+  <si>
+    <t>Handguard</t>
+  </si>
+  <si>
+    <t>WeaponBody</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>AKS-74U Body</t>
+  </si>
+  <si>
+    <t>Glock 19X Body</t>
+  </si>
+  <si>
+    <t>Zenit B-11</t>
+  </si>
+  <si>
+    <t>AKS-74U Skeleton ST</t>
+  </si>
+  <si>
+    <t>AKS-74U HG</t>
+  </si>
+  <si>
+    <t>AK-74 6L20 M</t>
+  </si>
+  <si>
+    <t>AK-74 6L31 M</t>
+  </si>
+  <si>
+    <t>Walther reflex S</t>
+  </si>
+  <si>
+    <t>Glock 19 19-M</t>
+  </si>
+  <si>
+    <t>Zenit-RK-3</t>
+  </si>
+  <si>
+    <t>AKS-74U Grip</t>
+  </si>
+  <si>
+    <t>KAC VG</t>
+  </si>
+  <si>
+    <t>AK-105 Muzzle B</t>
+  </si>
+  <si>
+    <t>AKS-74U LegalAP DC</t>
+  </si>
+  <si>
+    <t>Glock 19X Barrel</t>
+  </si>
+  <si>
+    <t>Glock 19X rear S</t>
+  </si>
+  <si>
+    <t>Glock 19X front S</t>
+  </si>
+  <si>
+    <t>Glock 19X slide</t>
+  </si>
+  <si>
+    <t>Olight Pro light/laser</t>
+  </si>
+  <si>
+    <t>AKS-74U_Body=AdvancedItems!A2</t>
+  </si>
+  <si>
+    <t>1;2;D</t>
+  </si>
+  <si>
+    <t>VerticalGrip</t>
+  </si>
+  <si>
+    <t>Magasine</t>
+  </si>
+  <si>
+    <t>MuzzleBreak</t>
+  </si>
+  <si>
+    <t>Sight</t>
+  </si>
+  <si>
+    <t>Stok</t>
+  </si>
+  <si>
+    <t>2;4;R</t>
+  </si>
+  <si>
+    <t>Barrel</t>
+  </si>
+  <si>
+    <t>5.45x39</t>
+  </si>
+  <si>
+    <t>Slide</t>
+  </si>
+  <si>
+    <t>Laser/Light</t>
+  </si>
+  <si>
+    <t>IsUsAble</t>
+  </si>
+  <si>
+    <t>ReloadAble</t>
+  </si>
+  <si>
+    <t>1.82</t>
+  </si>
+  <si>
+    <t>Cash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,18 +438,92 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -236,18 +531,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="5" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Bevitel" xfId="4" builtinId="20"/>
+    <cellStyle name="Ellenőrzőcella" xfId="5" builtinId="23"/>
+    <cellStyle name="Jó" xfId="1" builtinId="26"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Rossz" xfId="2" builtinId="27"/>
+    <cellStyle name="Semleges" xfId="3" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -460,11 +803,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J985"/>
+  <dimension ref="A1:J986"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -477,14 +818,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -509,14 +850,15 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
+      <c r="A2" s="3" t="str">
+        <f>AdvancedItems!A2</f>
+        <v>AKS-74U_Body</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -524,8 +866,9 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>45</v>
+      <c r="F2" t="str">
+        <f>AdvancedItems!A4 &amp; ";" &amp; AdvancedItems!A5</f>
+        <v>AKS-74U_Zenit_B-11_handguard;AKS-74U_Wooden_handguard</v>
       </c>
       <c r="G2" s="1">
         <v>205</v>
@@ -542,7 +885,7 @@
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -550,8 +893,9 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>29</v>
+      <c r="F3" s="3" t="str">
+        <f>AdvancedItems!A6</f>
+        <v>AKS-74U_Skeletonized_Stock</v>
       </c>
       <c r="G3" s="1">
         <v>535</v>
@@ -568,7 +912,7 @@
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
@@ -576,8 +920,9 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
+      <c r="F4" s="1" t="str">
+        <f>AdvancedItems!A7 &amp; ";" &amp; AdvancedItems!A8</f>
+        <v>AK-74_5.45x39_6L20_30-round_magasine;AK-74_5.45x39_6L31_60-round_magasine</v>
       </c>
       <c r="G4" s="1">
         <v>285</v>
@@ -594,7 +939,7 @@
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
@@ -602,8 +947,9 @@
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
+      <c r="F5" s="1" t="str">
+        <f>AdvancedItems!A10 &amp; ";" &amp; AdvancedItems!A11</f>
+        <v>AK_Zenit_RK-3_pistol_grip;AKS-74U_bakelite_pistol_grip</v>
       </c>
       <c r="G5" s="1">
         <v>453</v>
@@ -620,7 +966,7 @@
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>13</v>
@@ -628,8 +974,9 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
+      <c r="F6" s="1" t="str">
+        <f>AdvancedItems!A13</f>
+        <v>AK-105_5.45x39_muzzle_brake-compensator</v>
       </c>
       <c r="G6" s="1">
         <v>56</v>
@@ -646,16 +993,17 @@
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>19</v>
+      <c r="F7" s="2" t="str">
+        <f>AdvancedItems!A14 &amp; ";" &amp; AdvancedItems!A15</f>
+        <v>AKS-74U_dust_cover;AKS-74U_Legal_Arsenal_Pilgrim_railed_dust_cover</v>
       </c>
       <c r="G7" s="2">
         <v>312</v>
@@ -672,16 +1020,16 @@
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -697,14 +1045,15 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>20</v>
+      <c r="A9" s="3" t="str">
+        <f>AdvancedItems!A4</f>
+        <v>AKS-74U_Zenit_B-11_handguard</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
@@ -712,8 +1061,9 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>21</v>
+      <c r="F9" s="3" t="str">
+        <f>AdvancedItems!A2</f>
+        <v>AKS-74U_Body</v>
       </c>
       <c r="G9" s="1">
         <v>196</v>
@@ -730,7 +1080,7 @@
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
@@ -738,8 +1088,9 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>43</v>
+      <c r="F10" s="3" t="str">
+        <f>AdvancedItems!A12</f>
+        <v>KAC_vertical_foregrip</v>
       </c>
       <c r="G10" s="1">
         <v>62</v>
@@ -755,14 +1106,15 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>30</v>
+      <c r="A11" s="3" t="str">
+        <f>AdvancedItems!A5</f>
+        <v>AKS-74U_Wooden_handguard</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
@@ -770,8 +1122,9 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>21</v>
+      <c r="F11" s="3" t="str">
+        <f>AdvancedItems!A2</f>
+        <v>AKS-74U_Body</v>
       </c>
       <c r="G11" s="1">
         <v>215</v>
@@ -787,14 +1140,15 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>29</v>
+      <c r="A12" s="3" t="str">
+        <f>AdvancedItems!A6</f>
+        <v>AKS-74U_Skeletonized_Stock</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
@@ -802,8 +1156,9 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>21</v>
+      <c r="F12" s="3" t="str">
+        <f>AdvancedItems!A2</f>
+        <v>AKS-74U_Body</v>
       </c>
       <c r="G12" s="1">
         <v>62</v>
@@ -819,14 +1174,15 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>14</v>
+      <c r="A13" s="3" t="str">
+        <f>AdvancedItems!A7</f>
+        <v>AK-74_5.45x39_6L20_30-round_magasine</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
@@ -834,8 +1190,8 @@
       <c r="E13" s="1">
         <v>0</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>21</v>
+      <c r="F13" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="G13" s="1">
         <v>112</v>
@@ -851,14 +1207,15 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>22</v>
+      <c r="A14" s="3" t="str">
+        <f>AdvancedItems!A8</f>
+        <v>AK-74_5.45x39_6L31_60-round_magasine</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
@@ -866,8 +1223,9 @@
       <c r="E14" s="1">
         <v>0</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>21</v>
+      <c r="F14" s="1" t="str">
+        <f>AdvancedItems!A2</f>
+        <v>AKS-74U_Body</v>
       </c>
       <c r="G14" s="1">
         <v>103</v>
@@ -883,14 +1241,15 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>23</v>
+      <c r="A15" s="3" t="str">
+        <f>AdvancedItems!A10</f>
+        <v>AK_Zenit_RK-3_pistol_grip</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
@@ -898,8 +1257,9 @@
       <c r="E15" s="1">
         <v>0</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>21</v>
+      <c r="F15" s="1" t="str">
+        <f>AdvancedItems!A2</f>
+        <v>AKS-74U_Body</v>
       </c>
       <c r="G15" s="1">
         <v>21</v>
@@ -915,14 +1275,15 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>24</v>
+      <c r="A16" s="3" t="str">
+        <f>AdvancedItems!A11</f>
+        <v>AKS-74U_bakelite_pistol_grip</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
@@ -930,8 +1291,9 @@
       <c r="E16" s="1">
         <v>0</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>21</v>
+      <c r="F16" s="1" t="str">
+        <f>AdvancedItems!A2</f>
+        <v>AKS-74U_Body</v>
       </c>
       <c r="G16" s="1">
         <v>14</v>
@@ -947,14 +1309,15 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>43</v>
+      <c r="A17" s="3" t="str">
+        <f>AdvancedItems!A12</f>
+        <v>KAC_vertical_foregrip</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
@@ -962,8 +1325,9 @@
       <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>20</v>
+      <c r="F17" s="1" t="str">
+        <f>AdvancedItems!A4</f>
+        <v>AKS-74U_Zenit_B-11_handguard</v>
       </c>
       <c r="G17" s="1">
         <v>18</v>
@@ -979,14 +1343,15 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>18</v>
+      <c r="A18" s="3" t="str">
+        <f>AdvancedItems!A13</f>
+        <v>AK-105_5.45x39_muzzle_brake-compensator</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
@@ -994,8 +1359,9 @@
       <c r="E18" s="1">
         <v>0</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>21</v>
+      <c r="F18" s="1" t="str">
+        <f>AdvancedItems!A2</f>
+        <v>AKS-74U_Body</v>
       </c>
       <c r="G18" s="1">
         <v>138</v>
@@ -1011,14 +1377,15 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>25</v>
+      <c r="A19" t="str">
+        <f>AdvancedItems!A14</f>
+        <v>AKS-74U_dust_cover</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
@@ -1026,8 +1393,9 @@
       <c r="E19" s="2">
         <v>0</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>21</v>
+      <c r="F19" s="1" t="str">
+        <f>AdvancedItems!A2</f>
+        <v>AKS-74U_Body</v>
       </c>
       <c r="G19" s="2">
         <v>102</v>
@@ -1043,14 +1411,15 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>26</v>
+      <c r="A20" t="str">
+        <f>AdvancedItems!A15</f>
+        <v>AKS-74U_Legal_Arsenal_Pilgrim_railed_dust_cover</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
@@ -1058,8 +1427,9 @@
       <c r="E20" s="2">
         <v>0</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>21</v>
+      <c r="F20" s="1" t="str">
+        <f>AdvancedItems!A2</f>
+        <v>AKS-74U_Body</v>
       </c>
       <c r="G20" s="2">
         <v>105</v>
@@ -1076,7 +1446,7 @@
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>10</v>
@@ -1085,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G21" s="2">
         <v>180</v>
@@ -1101,14 +1471,15 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>27</v>
+      <c r="A22" t="str">
+        <f>AdvancedItems!A16</f>
+        <v>Walther_MRS_reflex_sight</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>9</v>
@@ -1116,8 +1487,9 @@
       <c r="E22" s="2">
         <v>0</v>
       </c>
-      <c r="F22" t="s">
-        <v>26</v>
+      <c r="F22" t="str">
+        <f>AdvancedItems!A16</f>
+        <v>Walther_MRS_reflex_sight</v>
       </c>
       <c r="G22" s="2">
         <v>6</v>
@@ -1132,32 +1504,418 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>AdvancedItems!A3</f>
+        <v>Glock_19X_9x19_pistol_body</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="str">
+        <f>AdvancedItems!A9</f>
+        <v>Glock_9x19_19-round_magasine_(Coyote)</v>
+      </c>
+      <c r="G23">
+        <v>358</v>
+      </c>
+      <c r="H23">
+        <v>304</v>
+      </c>
+      <c r="I23">
+        <v>460</v>
+      </c>
+      <c r="J23">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="str">
+        <f>AdvancedItems!A19</f>
+        <v>Glock_19X_9x19_barrel</v>
+      </c>
+      <c r="G24">
+        <v>200</v>
+      </c>
+      <c r="H24">
+        <v>31</v>
+      </c>
+      <c r="I24">
+        <v>267</v>
+      </c>
+      <c r="J24">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="str">
+        <f>AdvancedItems!A20</f>
+        <v>Glock_19X_pistol_slide</v>
+      </c>
+      <c r="G25">
+        <v>14</v>
+      </c>
+      <c r="H25">
+        <v>36</v>
+      </c>
+      <c r="I25">
+        <v>452</v>
+      </c>
+      <c r="J25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="str">
+        <f>AdvancedItems!A21</f>
+        <v>Olight_Baldr_Pro_tactical_flashlight_with_laser_(tan)</v>
+      </c>
+      <c r="G26">
+        <v>17</v>
+      </c>
+      <c r="H26">
+        <v>61</v>
+      </c>
+      <c r="I26">
+        <v>95</v>
+      </c>
+      <c r="J26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>AdvancedItems!A9</f>
+        <v>Glock_9x19_19-round_magasine_(Coyote)</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="str">
+        <f>AdvancedItems!A3</f>
+        <v>Glock_19X_9x19_pistol_body</v>
+      </c>
+      <c r="G27">
+        <v>60</v>
+      </c>
+      <c r="H27">
+        <v>183</v>
+      </c>
+      <c r="I27">
+        <v>121</v>
+      </c>
+      <c r="J27">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>AdvancedItems!A19</f>
+        <v>Glock_19X_9x19_barrel</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="str">
+        <f>AdvancedItems!A3</f>
+        <v>Glock_19X_9x19_pistol_body</v>
+      </c>
+      <c r="G28">
+        <v>202</v>
+      </c>
+      <c r="H28">
+        <v>68</v>
+      </c>
+      <c r="I28">
+        <v>267</v>
+      </c>
+      <c r="J28">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>AdvancedItems!A20</f>
+        <v>Glock_19X_pistol_slide</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="str">
+        <f>AdvancedItems!A3</f>
+        <v>Glock_19X_9x19_pistol_body</v>
+      </c>
+      <c r="G30">
+        <v>14</v>
+      </c>
+      <c r="H30">
+        <v>78</v>
+      </c>
+      <c r="I30">
+        <v>462</v>
+      </c>
+      <c r="J30">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="str">
+        <f>AdvancedItems!A17</f>
+        <v>Glock_19X_front_sight</v>
+      </c>
+      <c r="G31">
+        <v>25</v>
+      </c>
+      <c r="H31">
+        <v>22</v>
+      </c>
+      <c r="I31">
+        <v>55</v>
+      </c>
+      <c r="J31">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="str">
+        <f>AdvancedItems!A18</f>
+        <v>Glock_19X_rear_sight</v>
+      </c>
+      <c r="G32">
+        <v>425</v>
+      </c>
+      <c r="H32">
+        <v>25</v>
+      </c>
+      <c r="I32">
+        <v>443</v>
+      </c>
+      <c r="J32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>AdvancedItems!A17</f>
+        <v>Glock_19X_front_sight</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="str">
+        <f>AdvancedItems!A20</f>
+        <v>Glock_19X_pistol_slide</v>
+      </c>
+      <c r="G33">
+        <v>5</v>
+      </c>
+      <c r="H33">
+        <v>12</v>
+      </c>
+      <c r="I33">
+        <v>36</v>
+      </c>
+      <c r="J33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>AdvancedItems!A18</f>
+        <v>Glock_19X_rear_sight</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="str">
+        <f>AdvancedItems!A20</f>
+        <v>Glock_19X_pistol_slide</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="H34">
+        <v>21</v>
+      </c>
+      <c r="I34">
+        <v>23</v>
+      </c>
+      <c r="J34">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f>AdvancedItems!A21</f>
+        <v>Olight_Baldr_Pro_tactical_flashlight_with_laser_(tan)</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="str">
+        <f>AdvancedItems!A3</f>
+        <v>Glock_19X_9x19_pistol_body</v>
+      </c>
+      <c r="G35">
+        <v>83</v>
+      </c>
+      <c r="H35">
+        <v>8</v>
+      </c>
+      <c r="I35">
+        <v>159</v>
+      </c>
+      <c r="J35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2095,6 +2853,7 @@
     <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2106,54 +2865,58 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="29" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="29" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="str">
+        <f>System!A10</f>
+        <v>WeaponMain</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
+        <v>48</v>
+      </c>
+      <c r="E2" s="3" t="str">
+        <f>System!A5 &amp; ";" &amp; System!A7 &amp; ";" &amp; System!A8</f>
+        <v>Grip;Handguard;WeaponBody</v>
+      </c>
+      <c r="F2" t="str">
+        <f>AdvancedItems!A2</f>
+        <v>AKS-74U_Body</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3158,4 +3921,1443 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="14" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="9" t="str">
+        <f>System!A8</f>
+        <v>WeaponBody</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="9">
+        <v>2</v>
+      </c>
+      <c r="I2" s="9">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9">
+        <v>0</v>
+      </c>
+      <c r="L2" s="9">
+        <v>1</v>
+      </c>
+      <c r="M2" s="9">
+        <v>0</v>
+      </c>
+      <c r="N2" s="9">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9">
+        <v>1</v>
+      </c>
+      <c r="T2" s="9">
+        <v>1</v>
+      </c>
+      <c r="U2" s="9">
+        <v>800</v>
+      </c>
+      <c r="V2" s="9">
+        <v>1</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="X2" s="9">
+        <v>500</v>
+      </c>
+      <c r="Y2" s="9">
+        <v>52</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA2" s="9"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="9" t="str">
+        <f>System!A8</f>
+        <v>WeaponBody</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9">
+        <v>0</v>
+      </c>
+      <c r="L3" s="9">
+        <v>1</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0</v>
+      </c>
+      <c r="N3" s="9">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9">
+        <v>1</v>
+      </c>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="9" t="str">
+        <f>System!A7</f>
+        <v>Handguard</v>
+      </c>
+      <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9">
+        <v>1</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+      <c r="N4" s="9">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9">
+        <v>11</v>
+      </c>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="9" t="str">
+        <f>System!A7</f>
+        <v>Handguard</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9">
+        <v>1</v>
+      </c>
+      <c r="M5" s="9">
+        <v>0</v>
+      </c>
+      <c r="N5" s="9">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9">
+        <v>10</v>
+      </c>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="9" t="str">
+        <f>System!A11</f>
+        <v>Stok</v>
+      </c>
+      <c r="D6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
+        <v>2</v>
+      </c>
+      <c r="I6" s="9">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0</v>
+      </c>
+      <c r="L6" s="9">
+        <v>1</v>
+      </c>
+      <c r="M6" s="9">
+        <v>0</v>
+      </c>
+      <c r="N6" s="9">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="9" t="str">
+        <f>System!A3</f>
+        <v>Magasine</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>2</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9">
+        <v>1</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0</v>
+      </c>
+      <c r="N7" s="9">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9">
+        <v>30</v>
+      </c>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="9" t="str">
+        <f>System!A3</f>
+        <v>Magasine</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>2</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9">
+        <v>1</v>
+      </c>
+      <c r="M8" s="9">
+        <v>0</v>
+      </c>
+      <c r="N8" s="9">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9">
+        <v>60</v>
+      </c>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9">
+        <v>-5</v>
+      </c>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="9" t="str">
+        <f>System!A3</f>
+        <v>Magasine</v>
+      </c>
+      <c r="D9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="9">
+        <v>1</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9">
+        <v>19</v>
+      </c>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="9" t="str">
+        <f>System!A5</f>
+        <v>Grip</v>
+      </c>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9">
+        <v>1</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="K10" s="9">
+        <v>0</v>
+      </c>
+      <c r="L10" s="9">
+        <v>1</v>
+      </c>
+      <c r="M10" s="9">
+        <v>0</v>
+      </c>
+      <c r="N10" s="9">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="9" t="str">
+        <f>System!A5</f>
+        <v>Grip</v>
+      </c>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9">
+        <v>1</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
+        <v>1</v>
+      </c>
+      <c r="M11" s="9">
+        <v>0</v>
+      </c>
+      <c r="N11" s="9">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="9" t="str">
+        <f>System!A6</f>
+        <v>VerticalGrip</v>
+      </c>
+      <c r="D12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1</v>
+      </c>
+      <c r="I12" s="9">
+        <v>1</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9">
+        <v>0</v>
+      </c>
+      <c r="L12" s="9">
+        <v>1</v>
+      </c>
+      <c r="M12" s="9">
+        <v>0</v>
+      </c>
+      <c r="N12" s="9">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9">
+        <v>6</v>
+      </c>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="9" t="str">
+        <f>System!A2</f>
+        <v>MuzzleBreak</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9">
+        <v>1</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9">
+        <v>0</v>
+      </c>
+      <c r="L13" s="9">
+        <v>1</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0</v>
+      </c>
+      <c r="N13" s="9">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9">
+        <v>-2</v>
+      </c>
+      <c r="W13" s="9">
+        <v>10</v>
+      </c>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" t="str">
+        <f>System!A4</f>
+        <v>Dustcover</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0</v>
+      </c>
+      <c r="L14" s="9">
+        <v>1</v>
+      </c>
+      <c r="M14" s="9">
+        <v>0</v>
+      </c>
+      <c r="N14" s="9">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" t="str">
+        <f>System!A4</f>
+        <v>Dustcover</v>
+      </c>
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="K15" s="9">
+        <v>0</v>
+      </c>
+      <c r="L15" s="9">
+        <v>1</v>
+      </c>
+      <c r="M15" s="9">
+        <v>0</v>
+      </c>
+      <c r="N15" s="9">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" t="str">
+        <f>System!A9</f>
+        <v>Sight</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0</v>
+      </c>
+      <c r="L16" s="9">
+        <v>1</v>
+      </c>
+      <c r="M16" s="9">
+        <v>0</v>
+      </c>
+      <c r="N16" s="9">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>15</v>
+      </c>
+      <c r="Y16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" t="str">
+        <f>System!A9</f>
+        <v>Sight</v>
+      </c>
+      <c r="D17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0</v>
+      </c>
+      <c r="L17" s="9">
+        <v>1</v>
+      </c>
+      <c r="M17" s="9">
+        <v>0</v>
+      </c>
+      <c r="N17" s="9">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" t="str">
+        <f>System!A9</f>
+        <v>Sight</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9">
+        <v>1</v>
+      </c>
+      <c r="M18" s="9">
+        <v>0</v>
+      </c>
+      <c r="N18" s="9">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" t="str">
+        <f>System!A12</f>
+        <v>Barrel</v>
+      </c>
+      <c r="D19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0</v>
+      </c>
+      <c r="L19" s="9">
+        <v>1</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0</v>
+      </c>
+      <c r="N19" s="9">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="str">
+        <f>System!A13</f>
+        <v>Slide</v>
+      </c>
+      <c r="D20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="K20" s="9">
+        <v>0</v>
+      </c>
+      <c r="L20" s="9">
+        <v>1</v>
+      </c>
+      <c r="M20" s="9">
+        <v>0</v>
+      </c>
+      <c r="N20" s="9">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" t="str">
+        <f>System!A14</f>
+        <v>Laser/Light</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0</v>
+      </c>
+      <c r="L21" s="9">
+        <v>1</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0</v>
+      </c>
+      <c r="N21" s="9">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
V 0.1.7/q2 simple itemObject: removed from code , Inventory clone: updated , ItemCompond Refresh: replaced , Excel file loader full inplementation: completed
</commit_message>
<xml_diff>
--- a/Assets/Resources/Items/AdvancedItemData.xlsx
+++ b/Assets/Resources/Items/AdvancedItemData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="PartDatas" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,8 @@
     <sheet name="Stoks" sheetId="22" r:id="rId14"/>
     <sheet name="Magasines" sheetId="21" r:id="rId15"/>
     <sheet name="Armors" sheetId="5" r:id="rId16"/>
-    <sheet name="Backpacks" sheetId="6" r:id="rId17"/>
-    <sheet name="Boots" sheetId="7" r:id="rId18"/>
+    <sheet name="Boots" sheetId="7" r:id="rId17"/>
+    <sheet name="Backpacks" sheetId="6" r:id="rId18"/>
     <sheet name="Cash" sheetId="8" r:id="rId19"/>
     <sheet name="Fingers" sheetId="9" r:id="rId20"/>
     <sheet name="Headsets" sheetId="10" r:id="rId21"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1773" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="599">
   <si>
     <t>PartName</t>
   </si>
@@ -1838,6 +1838,12 @@
   </si>
   <si>
     <t>AKS-74U HG</t>
+  </si>
+  <si>
+    <t>GameElements/ItemContainers/Backpacks/TestBackpack</t>
+  </si>
+  <si>
+    <t>GameElements/ItemContainers/Vests/TestVest</t>
   </si>
 </sst>
 </file>
@@ -2234,7 +2240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J986"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -8835,8 +8841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10205,684 +10211,6 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AA2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
-    <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" customWidth="1"/>
-    <col min="25" max="25" width="13.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C2" t="str">
-        <f>System!A16</f>
-        <v>Backpack</v>
-      </c>
-      <c r="D2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" t="str">
-        <f>System!A16</f>
-        <v>Backpack</v>
-      </c>
-      <c r="D3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C4" t="str">
-        <f>System!A16</f>
-        <v>Backpack</v>
-      </c>
-      <c r="D4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>4</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="C5" t="str">
-        <f>System!A16</f>
-        <v>Backpack</v>
-      </c>
-      <c r="D5" t="s">
-        <v>174</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C6" t="str">
-        <f>System!A16</f>
-        <v>Backpack</v>
-      </c>
-      <c r="D6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" t="str">
-        <f>System!A16</f>
-        <v>Backpack</v>
-      </c>
-      <c r="D7" t="s">
-        <v>174</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>4</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>182</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C8" t="str">
-        <f>System!A16</f>
-        <v>Backpack</v>
-      </c>
-      <c r="D8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C9" t="str">
-        <f>System!A16</f>
-        <v>Backpack</v>
-      </c>
-      <c r="D9" t="s">
-        <v>176</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>188</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C10" t="str">
-        <f>System!A16</f>
-        <v>Backpack</v>
-      </c>
-      <c r="D10" t="s">
-        <v>176</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>4</v>
-      </c>
-      <c r="I10">
-        <v>4</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="C11" t="str">
-        <f>System!A16</f>
-        <v>Backpack</v>
-      </c>
-      <c r="D11" t="s">
-        <v>176</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>4</v>
-      </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>192</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C12" t="str">
-        <f>System!A16</f>
-        <v>Backpack</v>
-      </c>
-      <c r="D12" t="s">
-        <v>174</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>4</v>
-      </c>
-      <c r="I12">
-        <v>5</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11041,6 +10369,687 @@
         <v>0</v>
       </c>
       <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="18" max="18" width="14" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" customWidth="1"/>
+    <col min="25" max="25" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" t="str">
+        <f>System!A16</f>
+        <v>Backpack</v>
+      </c>
+      <c r="D2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" t="str">
+        <f>System!A16</f>
+        <v>Backpack</v>
+      </c>
+      <c r="D3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" t="str">
+        <f>System!A16</f>
+        <v>Backpack</v>
+      </c>
+      <c r="D4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" t="str">
+        <f>System!A16</f>
+        <v>Backpack</v>
+      </c>
+      <c r="D5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" t="str">
+        <f>System!A16</f>
+        <v>Backpack</v>
+      </c>
+      <c r="D6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" t="str">
+        <f>System!A16</f>
+        <v>Backpack</v>
+      </c>
+      <c r="D7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" t="str">
+        <f>System!A16</f>
+        <v>Backpack</v>
+      </c>
+      <c r="D8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" t="str">
+        <f>System!A16</f>
+        <v>Backpack</v>
+      </c>
+      <c r="D9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" t="str">
+        <f>System!A16</f>
+        <v>Backpack</v>
+      </c>
+      <c r="D10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" t="str">
+        <f>System!A16</f>
+        <v>Backpack</v>
+      </c>
+      <c r="D11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" t="str">
+        <f>System!A16</f>
+        <v>Backpack</v>
+      </c>
+      <c r="D12" t="s">
+        <v>174</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
         <v>0</v>
       </c>
     </row>
@@ -16525,7 +16534,7 @@
   <dimension ref="A1:AA12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AA2"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16681,6 +16690,9 @@
       </c>
       <c r="Q2">
         <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
V 0.1.7/r2 SystemPoints: added and completed
</commit_message>
<xml_diff>
--- a/Assets/Resources/Items/AdvancedItemData.xlsx
+++ b/Assets/Resources/Items/AdvancedItemData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="PartDatas" sheetId="1" r:id="rId1"/>
@@ -2240,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J986"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2469,16 +2469,16 @@
         <v>52</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8841,7 +8841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
V 0.1.7/t2 Excel File Reader inplemented to the Main
</commit_message>
<xml_diff>
--- a/Assets/Resources/Items/AdvancedItemData.xlsx
+++ b/Assets/Resources/Items/AdvancedItemData.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1944" uniqueCount="616">
   <si>
     <t>PartName</t>
   </si>
@@ -1852,16 +1852,49 @@
     <t>MuzzleVelocity</t>
   </si>
   <si>
-    <t>WeaponTypes</t>
-  </si>
-  <si>
-    <t>WeaponMain</t>
-  </si>
-  <si>
-    <t>Handgun</t>
-  </si>
-  <si>
     <t>Melee</t>
+  </si>
+  <si>
+    <t>Revolver</t>
+  </si>
+  <si>
+    <t>Pistol</t>
+  </si>
+  <si>
+    <t>Rifle</t>
+  </si>
+  <si>
+    <t>ShotGun</t>
+  </si>
+  <si>
+    <t>Carbine</t>
+  </si>
+  <si>
+    <t>AssaultRifle</t>
+  </si>
+  <si>
+    <t>BattleRifle</t>
+  </si>
+  <si>
+    <t>SniperRifle</t>
+  </si>
+  <si>
+    <t>AutomaticRifle</t>
+  </si>
+  <si>
+    <t>MachineGun</t>
+  </si>
+  <si>
+    <t>SMG</t>
+  </si>
+  <si>
+    <t>PDW</t>
+  </si>
+  <si>
+    <t>MainWeapons</t>
+  </si>
+  <si>
+    <t>SecondaryWeapons</t>
   </si>
 </sst>
 </file>
@@ -9327,8 +9360,8 @@
         <v>96</v>
       </c>
       <c r="C2" t="str">
-        <f>System!B3</f>
-        <v>Handgun</v>
+        <f>System!D3</f>
+        <v>Pistol</v>
       </c>
       <c r="D2" t="s">
         <v>93</v>
@@ -9694,7 +9727,7 @@
   <dimension ref="A1:AG12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AG1"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10286,8 +10319,8 @@
         <v>153</v>
       </c>
       <c r="C11" t="str">
-        <f>Backpacks!C2</f>
-        <v>Backpack</v>
+        <f>System!A13</f>
+        <v>Armor</v>
       </c>
       <c r="D11" t="s">
         <v>148</v>
@@ -11485,15 +11518,15 @@
         <v>39</v>
       </c>
       <c r="C2" t="str">
-        <f>System!B2</f>
-        <v>WeaponMain</v>
+        <f>System!C4</f>
+        <v>Carbine</v>
       </c>
       <c r="D2" t="s">
         <v>45</v>
       </c>
       <c r="E2" t="str">
-        <f>System!A5 &amp; ";" &amp; System!B3 &amp; ";" &amp; System!A7</f>
-        <v>Grip;Handgun;WeaponBody</v>
+        <f>System!A5 &amp; ";" &amp; System!D3 &amp; ";" &amp; System!A7</f>
+        <v>Grip;Pistol;WeaponBody</v>
       </c>
       <c r="F2" t="str">
         <f>WeaponBodies!A2</f>
@@ -14820,7 +14853,7 @@
   <dimension ref="A1:AG12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AG1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14953,7 +14986,7 @@
         <v>339</v>
       </c>
       <c r="C2" t="str">
-        <f>System!B4</f>
+        <f>System!B2</f>
         <v>Melee</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -15004,7 +15037,7 @@
         <v>342</v>
       </c>
       <c r="C3" t="str">
-        <f>System!B4</f>
+        <f>System!B2</f>
         <v>Melee</v>
       </c>
       <c r="D3" t="s">
@@ -15055,7 +15088,7 @@
         <v>345</v>
       </c>
       <c r="C4" t="str">
-        <f>System!B4</f>
+        <f>System!B2</f>
         <v>Melee</v>
       </c>
       <c r="D4" t="s">
@@ -15106,7 +15139,7 @@
         <v>348</v>
       </c>
       <c r="C5" t="str">
-        <f>System!B4</f>
+        <f>System!B2</f>
         <v>Melee</v>
       </c>
       <c r="D5" t="s">
@@ -15157,7 +15190,7 @@
         <v>351</v>
       </c>
       <c r="C6" t="str">
-        <f>System!B4</f>
+        <f>System!B2</f>
         <v>Melee</v>
       </c>
       <c r="D6" t="s">
@@ -15208,7 +15241,7 @@
         <v>354</v>
       </c>
       <c r="C7" t="str">
-        <f>System!B4</f>
+        <f>System!B2</f>
         <v>Melee</v>
       </c>
       <c r="D7" t="s">
@@ -15259,7 +15292,7 @@
         <v>357</v>
       </c>
       <c r="C8" t="str">
-        <f>System!B4</f>
+        <f>System!B2</f>
         <v>Melee</v>
       </c>
       <c r="D8" t="s">
@@ -15310,7 +15343,7 @@
         <v>360</v>
       </c>
       <c r="C9" t="str">
-        <f>System!B4</f>
+        <f>System!B2</f>
         <v>Melee</v>
       </c>
       <c r="D9" t="s">
@@ -15361,7 +15394,7 @@
         <v>363</v>
       </c>
       <c r="C10" t="str">
-        <f>System!B4</f>
+        <f>System!B2</f>
         <v>Melee</v>
       </c>
       <c r="D10" t="s">
@@ -15412,7 +15445,7 @@
         <v>366</v>
       </c>
       <c r="C11" t="str">
-        <f>System!B4</f>
+        <f>System!B2</f>
         <v>Melee</v>
       </c>
       <c r="D11" t="s">
@@ -15463,7 +15496,7 @@
         <v>369</v>
       </c>
       <c r="C12" t="str">
-        <f>System!B4</f>
+        <f>System!B2</f>
         <v>Melee</v>
       </c>
       <c r="D12" t="s">
@@ -18983,151 +19016,192 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>114</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>601</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>604</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="13" t="s">
+        <v>605</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="13" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="13" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="13" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="13" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="13" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="13" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="13" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="13" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="13"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="13"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>483</v>
       </c>

</xml_diff>

<commit_message>
V 0.1.7/x2 InGame ItemCompound Handling: completed , SimpleItem and AdvancedItem: completed , Some Componens: updated
</commit_message>
<xml_diff>
--- a/Assets/Resources/Items/AdvancedItemData.xlsx
+++ b/Assets/Resources/Items/AdvancedItemData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="19" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="PartDatas" sheetId="1" r:id="rId1"/>
@@ -2099,8 +2099,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="5" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="5" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
@@ -17641,8 +17641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17818,20 +17818,20 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="AC2" s="11">
-        <v>0</v>
+      <c r="AC2" s="13">
+        <v>7.62</v>
       </c>
       <c r="AD2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="11">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="AF2" s="13">
+        <v>0.08</v>
       </c>
       <c r="AG2">
-        <v>0</v>
+        <v>730</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
@@ -19018,7 +19018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -19034,13 +19034,13 @@
       <c r="A1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>601</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>614</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>615</v>
       </c>
     </row>
@@ -19048,13 +19048,13 @@
       <c r="A2" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>601</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>604</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>602</v>
       </c>
     </row>
@@ -19062,10 +19062,10 @@
       <c r="A3" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>605</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>603</v>
       </c>
     </row>
@@ -19073,7 +19073,7 @@
       <c r="A4" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>606</v>
       </c>
     </row>
@@ -19081,7 +19081,7 @@
       <c r="A5" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>607</v>
       </c>
     </row>
@@ -19089,7 +19089,7 @@
       <c r="A6" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>608</v>
       </c>
     </row>
@@ -19097,7 +19097,7 @@
       <c r="A7" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>609</v>
       </c>
     </row>
@@ -19105,7 +19105,7 @@
       <c r="A8" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>610</v>
       </c>
     </row>
@@ -19113,7 +19113,7 @@
       <c r="A9" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>611</v>
       </c>
     </row>
@@ -19121,7 +19121,7 @@
       <c r="A10" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>612</v>
       </c>
     </row>
@@ -19129,7 +19129,7 @@
       <c r="A11" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>613</v>
       </c>
     </row>
@@ -19162,13 +19162,13 @@
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="13"/>
+      <c r="B17" s="12"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="B18" s="13"/>
+      <c r="B18" s="12"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
@@ -19179,7 +19179,7 @@
       <c r="A20" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="B20" s="13"/>
+      <c r="B20" s="12"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">

</xml_diff>

<commit_message>
V 0.1.7/y2 Weapons sound added
</commit_message>
<xml_diff>
--- a/Assets/Resources/Items/AdvancedItemData.xlsx
+++ b/Assets/Resources/Items/AdvancedItemData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="19" activeTab="28"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PartDatas" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1944" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1945" uniqueCount="617">
   <si>
     <t>PartName</t>
   </si>
@@ -1895,17 +1895,28 @@
   </si>
   <si>
     <t>SecondaryWeapons</t>
+  </si>
+  <si>
+    <t>HandGuard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2081,25 +2092,26 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="5" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="4" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="5" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="5" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="5" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="5" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="5" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -11478,8 +11490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11525,8 +11537,8 @@
         <v>45</v>
       </c>
       <c r="E2" t="str">
-        <f>System!A5 &amp; ";" &amp; System!D3 &amp; ";" &amp; System!A7</f>
-        <v>Grip;Pistol;WeaponBody</v>
+        <f>System!A5 &amp; ";" &amp; System!A26 &amp; ";" &amp; System!A7</f>
+        <v>Grip;HandGuard;WeaponBody</v>
       </c>
       <c r="F2" t="str">
         <f>WeaponBodies!A2</f>
@@ -14843,7 +14855,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16236,7 +16248,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -17632,7 +17644,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -17641,7 +17653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
@@ -19008,7 +19020,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -19016,10 +19028,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19204,6 +19216,11 @@
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>483</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>616</v>
       </c>
     </row>
   </sheetData>
@@ -19479,7 +19496,7 @@
   <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AG1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19611,8 +19628,8 @@
         <v>591</v>
       </c>
       <c r="C2" t="str">
-        <f>System!A5</f>
-        <v>Grip</v>
+        <f>System!A26</f>
+        <v>HandGuard</v>
       </c>
       <c r="D2" t="s">
         <v>93</v>
@@ -19665,8 +19682,8 @@
         <v>593</v>
       </c>
       <c r="C3" t="str">
-        <f>System!A5</f>
-        <v>Grip</v>
+        <f>System!A26</f>
+        <v>HandGuard</v>
       </c>
       <c r="D3" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
V 0.1.8/d Weapon Layered Part positioning: completed , new main item added: Glock19X with parts but it is currently nonUsable
</commit_message>
<xml_diff>
--- a/Assets/Resources/Items/AdvancedItemData.xlsx
+++ b/Assets/Resources/Items/AdvancedItemData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PartDatas" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1957" uniqueCount="627">
   <si>
     <t>PartName</t>
   </si>
@@ -1922,6 +1922,12 @@
   </si>
   <si>
     <t>Sounds/WeaponTEST/TESTReload</t>
+  </si>
+  <si>
+    <t>Glock-19X</t>
+  </si>
+  <si>
+    <t>an iconic variant of the glock series</t>
   </si>
 </sst>
 </file>
@@ -2401,7 +2407,7 @@
   <dimension ref="A1:J986"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3118,7 +3124,7 @@
         <v>9</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F23" t="str">
         <f>Magasines!A4</f>
@@ -3145,7 +3151,7 @@
         <v>10</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F24" t="str">
         <f>Barrels!A2</f>
@@ -3172,7 +3178,7 @@
         <v>11</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" t="str">
         <f>Slides!A2</f>
@@ -3300,16 +3306,16 @@
         <v>51</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11560,8 +11566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11650,7 +11656,27 @@
         <v>620</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>625</v>
+      </c>
+      <c r="B3" t="s">
+        <v>625</v>
+      </c>
+      <c r="C3" t="s">
+        <v>610</v>
+      </c>
+      <c r="D3" t="s">
+        <v>626</v>
+      </c>
+      <c r="E3" t="str">
+        <f>System!D5 &amp; ";" &amp; System!D4 &amp; ";" &amp; System!D8</f>
+        <v>Barrel;Slide;WeaponBody</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19335,8 +19361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1:AI1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19591,6 +19617,30 @@
       </c>
       <c r="S3">
         <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>600</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>150</v>
+      </c>
+      <c r="Y3">
+        <v>75</v>
+      </c>
+      <c r="AB3">
+        <v>9</v>
+      </c>
+      <c r="AC3">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -20322,8 +20372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1:AI1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20507,8 +20557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1:AI1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
V 0.1.8/e Glock19X: ready to Operate
</commit_message>
<xml_diff>
--- a/Assets/Resources/Items/AdvancedItemData.xlsx
+++ b/Assets/Resources/Items/AdvancedItemData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PartDatas" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1957" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="632">
   <si>
     <t>PartName</t>
   </si>
@@ -1928,6 +1928,21 @@
   </si>
   <si>
     <t>an iconic variant of the glock series</t>
+  </si>
+  <si>
+    <t>Textures/EffectTextures/9mmBullet</t>
+  </si>
+  <si>
+    <t>Sounds/Glock/GlockChamber</t>
+  </si>
+  <si>
+    <t>Sounds/Glock/GlockReload</t>
+  </si>
+  <si>
+    <t>Sounds/Glock/GlockShoot</t>
+  </si>
+  <si>
+    <t>Sounds/Glock/GlockUnload</t>
   </si>
 </sst>
 </file>
@@ -11566,8 +11581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11675,6 +11690,21 @@
       </c>
       <c r="F3" t="s">
         <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>630</v>
+      </c>
+      <c r="H3" t="s">
+        <v>629</v>
+      </c>
+      <c r="I3" t="s">
+        <v>631</v>
+      </c>
+      <c r="J3" t="s">
+        <v>628</v>
+      </c>
+      <c r="K3" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17787,8 +17817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection sqref="A1:AG1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18339,6 +18369,24 @@
       <c r="Q9">
         <v>0</v>
       </c>
+      <c r="AB9">
+        <v>9</v>
+      </c>
+      <c r="AC9">
+        <v>19</v>
+      </c>
+      <c r="AD9">
+        <v>4</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AG9">
+        <v>450</v>
+      </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -19361,7 +19409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>

</xml_diff>